<commit_message>
1061685 - Pagero X12 810 Invoice - Updated Specifications with header note
</commit_message>
<xml_diff>
--- a/format-specifications/ansi-x12/4010/810/Pagero-ANSI-X12-4010-810-invoice-description-outbound.xlsx
+++ b/format-specifications/ansi-x12/4010/810/Pagero-ANSI-X12-4010-810-invoice-description-outbound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\integration-resources\format-specifications\ansi-x12\4010\810\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA1026-73E8-4D95-92AE-595B01A222DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EA0FBE-8B7B-413B-92D1-16A733BC1B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="0" windowWidth="27150" windowHeight="21165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="574">
   <si>
     <t>Responsible</t>
   </si>
@@ -1912,7 +1912,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2065,6 +2065,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2079,7 +2103,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2362,6 +2386,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2414,12 +2450,6 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -2428,24 +2458,6 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2465,15 +2477,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2969,90 +3005,90 @@
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="99"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="102"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="102"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="105"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="106" t="s">
         <v>494</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="105"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="108"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="111"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="108"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="111"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="107"/>
-      <c r="D13" s="108"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="108"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="111"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="107"/>
-      <c r="D15" s="108"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
-      <c r="B16" s="106"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="108"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="111"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="108"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="110"/>
+      <c r="D17" s="111"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
-      <c r="B18" s="106"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="108"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="111"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="111"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="114"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
@@ -3064,18 +3100,18 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2"/>
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2"/>
-      <c r="B22" s="112"/>
-      <c r="C22" s="112"/>
-      <c r="D22" s="112"/>
+      <c r="B22" s="115"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
@@ -3201,9 +3237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G156" sqref="G156"/>
+      <selection pane="bottomLeft" activeCell="A154" sqref="A154:XFD160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3637,14 +3673,14 @@
       <c r="A20" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B20" s="127" t="s">
+      <c r="B20" s="122" t="s">
         <v>314</v>
       </c>
-      <c r="C20" s="128"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="128"/>
-      <c r="F20" s="128"/>
-      <c r="G20" s="129"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="124"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="35"/>
@@ -3856,14 +3892,14 @@
       <c r="A31" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B31" s="113" t="s">
+      <c r="B31" s="116" t="s">
         <v>336</v>
       </c>
-      <c r="C31" s="114"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="115"/>
+      <c r="C31" s="125"/>
+      <c r="D31" s="125"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="125"/>
+      <c r="G31" s="126"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="28"/>
@@ -3939,14 +3975,14 @@
       <c r="A36" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="113" t="s">
+      <c r="B36" s="116" t="s">
         <v>340</v>
       </c>
-      <c r="C36" s="114"/>
-      <c r="D36" s="114"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="115"/>
+      <c r="C36" s="125"/>
+      <c r="D36" s="125"/>
+      <c r="E36" s="125"/>
+      <c r="F36" s="125"/>
+      <c r="G36" s="126"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="28"/>
@@ -4191,25 +4227,25 @@
       <c r="A49" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B49" s="113" t="s">
+      <c r="B49" s="116" t="s">
         <v>351</v>
       </c>
-      <c r="C49" s="114"/>
-      <c r="D49" s="114"/>
-      <c r="E49" s="114"/>
-      <c r="F49" s="114"/>
-      <c r="G49" s="115"/>
+      <c r="C49" s="125"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="125"/>
+      <c r="F49" s="125"/>
+      <c r="G49" s="126"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="28"/>
-      <c r="B50" s="113" t="s">
+      <c r="B50" s="116" t="s">
         <v>399</v>
       </c>
-      <c r="C50" s="114"/>
-      <c r="D50" s="114"/>
-      <c r="E50" s="114"/>
-      <c r="F50" s="114"/>
-      <c r="G50" s="115"/>
+      <c r="C50" s="125"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="125"/>
+      <c r="F50" s="125"/>
+      <c r="G50" s="126"/>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="28"/>
@@ -4411,13 +4447,13 @@
       <c r="A61" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B61" s="122" t="s">
+      <c r="B61" s="131" t="s">
         <v>553</v>
       </c>
-      <c r="C61" s="123"/>
-      <c r="D61" s="123"/>
-      <c r="E61" s="123"/>
-      <c r="F61" s="123"/>
+      <c r="C61" s="132"/>
+      <c r="D61" s="132"/>
+      <c r="E61" s="132"/>
+      <c r="F61" s="132"/>
       <c r="G61" s="96" t="s">
         <v>554</v>
       </c>
@@ -4426,14 +4462,14 @@
       <c r="A62" s="35" t="s">
         <v>552</v>
       </c>
-      <c r="B62" s="121" t="s">
+      <c r="B62" s="130" t="s">
         <v>511</v>
       </c>
-      <c r="C62" s="114"/>
-      <c r="D62" s="114"/>
-      <c r="E62" s="114"/>
-      <c r="F62" s="114"/>
-      <c r="G62" s="115"/>
+      <c r="C62" s="125"/>
+      <c r="D62" s="125"/>
+      <c r="E62" s="125"/>
+      <c r="F62" s="125"/>
+      <c r="G62" s="126"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="77"/>
@@ -4505,14 +4541,14 @@
       <c r="A67" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B67" s="113" t="s">
+      <c r="B67" s="116" t="s">
         <v>355</v>
       </c>
-      <c r="C67" s="114"/>
-      <c r="D67" s="114"/>
-      <c r="E67" s="114"/>
-      <c r="F67" s="114"/>
-      <c r="G67" s="115"/>
+      <c r="C67" s="125"/>
+      <c r="D67" s="125"/>
+      <c r="E67" s="125"/>
+      <c r="F67" s="125"/>
+      <c r="G67" s="126"/>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="51"/>
@@ -4584,14 +4620,14 @@
       <c r="A72" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B72" s="113" t="s">
+      <c r="B72" s="116" t="s">
         <v>357</v>
       </c>
-      <c r="C72" s="114"/>
-      <c r="D72" s="114"/>
-      <c r="E72" s="114"/>
-      <c r="F72" s="114"/>
-      <c r="G72" s="115"/>
+      <c r="C72" s="125"/>
+      <c r="D72" s="125"/>
+      <c r="E72" s="125"/>
+      <c r="F72" s="125"/>
+      <c r="G72" s="126"/>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="51"/>
@@ -4663,14 +4699,14 @@
       <c r="A77" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B77" s="113" t="s">
+      <c r="B77" s="116" t="s">
         <v>359</v>
       </c>
-      <c r="C77" s="114"/>
-      <c r="D77" s="114"/>
-      <c r="E77" s="114"/>
-      <c r="F77" s="114"/>
-      <c r="G77" s="115"/>
+      <c r="C77" s="125"/>
+      <c r="D77" s="125"/>
+      <c r="E77" s="125"/>
+      <c r="F77" s="125"/>
+      <c r="G77" s="126"/>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="40"/>
@@ -4742,14 +4778,14 @@
       <c r="A82" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B82" s="113" t="s">
+      <c r="B82" s="116" t="s">
         <v>432</v>
       </c>
-      <c r="C82" s="114"/>
-      <c r="D82" s="114"/>
-      <c r="E82" s="114"/>
-      <c r="F82" s="114"/>
-      <c r="G82" s="115"/>
+      <c r="C82" s="125"/>
+      <c r="D82" s="125"/>
+      <c r="E82" s="125"/>
+      <c r="F82" s="125"/>
+      <c r="G82" s="126"/>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="35"/>
@@ -4911,25 +4947,25 @@
       <c r="A91" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B91" s="113" t="s">
+      <c r="B91" s="116" t="s">
         <v>421</v>
       </c>
-      <c r="C91" s="116"/>
-      <c r="D91" s="116"/>
-      <c r="E91" s="116"/>
-      <c r="F91" s="116"/>
-      <c r="G91" s="117"/>
+      <c r="C91" s="117"/>
+      <c r="D91" s="117"/>
+      <c r="E91" s="117"/>
+      <c r="F91" s="117"/>
+      <c r="G91" s="118"/>
     </row>
     <row r="92" spans="1:7" ht="12.75" customHeight="1">
       <c r="A92" s="28"/>
-      <c r="B92" s="113" t="s">
+      <c r="B92" s="116" t="s">
         <v>422</v>
       </c>
-      <c r="C92" s="116"/>
-      <c r="D92" s="116"/>
-      <c r="E92" s="116"/>
-      <c r="F92" s="116"/>
-      <c r="G92" s="117"/>
+      <c r="C92" s="117"/>
+      <c r="D92" s="117"/>
+      <c r="E92" s="117"/>
+      <c r="F92" s="117"/>
+      <c r="G92" s="118"/>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="28"/>
@@ -5250,135 +5286,135 @@
       <c r="A110" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B110" s="118" t="s">
+      <c r="B110" s="127" t="s">
         <v>365</v>
       </c>
-      <c r="C110" s="119"/>
-      <c r="D110" s="119"/>
-      <c r="E110" s="119"/>
-      <c r="F110" s="119"/>
-      <c r="G110" s="120"/>
+      <c r="C110" s="128"/>
+      <c r="D110" s="128"/>
+      <c r="E110" s="128"/>
+      <c r="F110" s="128"/>
+      <c r="G110" s="129"/>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="40"/>
-      <c r="B111" s="118" t="s">
+      <c r="B111" s="127" t="s">
         <v>376</v>
       </c>
-      <c r="C111" s="119"/>
-      <c r="D111" s="119"/>
-      <c r="E111" s="119"/>
-      <c r="F111" s="119"/>
-      <c r="G111" s="120"/>
+      <c r="C111" s="128"/>
+      <c r="D111" s="128"/>
+      <c r="E111" s="128"/>
+      <c r="F111" s="128"/>
+      <c r="G111" s="129"/>
     </row>
     <row r="112" spans="1:7" ht="12.75" customHeight="1">
       <c r="A112" s="40"/>
-      <c r="B112" s="118" t="s">
+      <c r="B112" s="127" t="s">
         <v>377</v>
       </c>
-      <c r="C112" s="119"/>
-      <c r="D112" s="119"/>
-      <c r="E112" s="119"/>
-      <c r="F112" s="119"/>
-      <c r="G112" s="120"/>
+      <c r="C112" s="128"/>
+      <c r="D112" s="128"/>
+      <c r="E112" s="128"/>
+      <c r="F112" s="128"/>
+      <c r="G112" s="129"/>
     </row>
     <row r="113" spans="1:7" ht="12.75" customHeight="1">
       <c r="A113" s="40"/>
-      <c r="B113" s="118" t="s">
+      <c r="B113" s="127" t="s">
         <v>482</v>
       </c>
-      <c r="C113" s="119"/>
-      <c r="D113" s="119"/>
-      <c r="E113" s="119"/>
-      <c r="F113" s="119"/>
-      <c r="G113" s="120"/>
+      <c r="C113" s="128"/>
+      <c r="D113" s="128"/>
+      <c r="E113" s="128"/>
+      <c r="F113" s="128"/>
+      <c r="G113" s="129"/>
     </row>
     <row r="114" spans="1:7" ht="12.75" customHeight="1">
       <c r="A114" s="40"/>
-      <c r="B114" s="118" t="s">
+      <c r="B114" s="127" t="s">
         <v>366</v>
       </c>
-      <c r="C114" s="119"/>
-      <c r="D114" s="119"/>
-      <c r="E114" s="119"/>
-      <c r="F114" s="119"/>
-      <c r="G114" s="120"/>
+      <c r="C114" s="128"/>
+      <c r="D114" s="128"/>
+      <c r="E114" s="128"/>
+      <c r="F114" s="128"/>
+      <c r="G114" s="129"/>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="40"/>
-      <c r="B115" s="118" t="s">
+      <c r="B115" s="127" t="s">
         <v>376</v>
       </c>
-      <c r="C115" s="119"/>
-      <c r="D115" s="119"/>
-      <c r="E115" s="119"/>
-      <c r="F115" s="119"/>
-      <c r="G115" s="120"/>
+      <c r="C115" s="128"/>
+      <c r="D115" s="128"/>
+      <c r="E115" s="128"/>
+      <c r="F115" s="128"/>
+      <c r="G115" s="129"/>
     </row>
     <row r="116" spans="1:7" ht="12.75" customHeight="1">
       <c r="A116" s="40"/>
-      <c r="B116" s="118" t="s">
+      <c r="B116" s="127" t="s">
         <v>378</v>
       </c>
-      <c r="C116" s="119"/>
-      <c r="D116" s="119"/>
-      <c r="E116" s="119"/>
-      <c r="F116" s="119"/>
-      <c r="G116" s="120"/>
+      <c r="C116" s="128"/>
+      <c r="D116" s="128"/>
+      <c r="E116" s="128"/>
+      <c r="F116" s="128"/>
+      <c r="G116" s="129"/>
     </row>
     <row r="117" spans="1:7" ht="12.75" customHeight="1">
       <c r="A117" s="40"/>
-      <c r="B117" s="118" t="s">
+      <c r="B117" s="127" t="s">
         <v>483</v>
       </c>
-      <c r="C117" s="119"/>
-      <c r="D117" s="119"/>
-      <c r="E117" s="119"/>
-      <c r="F117" s="119"/>
-      <c r="G117" s="120"/>
+      <c r="C117" s="128"/>
+      <c r="D117" s="128"/>
+      <c r="E117" s="128"/>
+      <c r="F117" s="128"/>
+      <c r="G117" s="129"/>
     </row>
     <row r="118" spans="1:7" ht="12.75" customHeight="1">
       <c r="A118" s="40"/>
-      <c r="B118" s="118" t="s">
+      <c r="B118" s="127" t="s">
         <v>367</v>
       </c>
-      <c r="C118" s="119"/>
-      <c r="D118" s="119"/>
-      <c r="E118" s="119"/>
-      <c r="F118" s="119"/>
-      <c r="G118" s="120"/>
+      <c r="C118" s="128"/>
+      <c r="D118" s="128"/>
+      <c r="E118" s="128"/>
+      <c r="F118" s="128"/>
+      <c r="G118" s="129"/>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="28"/>
-      <c r="B119" s="113" t="s">
+      <c r="B119" s="116" t="s">
         <v>376</v>
       </c>
-      <c r="C119" s="116"/>
-      <c r="D119" s="116"/>
-      <c r="E119" s="116"/>
-      <c r="F119" s="116"/>
-      <c r="G119" s="117"/>
+      <c r="C119" s="117"/>
+      <c r="D119" s="117"/>
+      <c r="E119" s="117"/>
+      <c r="F119" s="117"/>
+      <c r="G119" s="118"/>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="28"/>
-      <c r="B120" s="113" t="s">
+      <c r="B120" s="116" t="s">
         <v>379</v>
       </c>
-      <c r="C120" s="116"/>
-      <c r="D120" s="116"/>
-      <c r="E120" s="116"/>
-      <c r="F120" s="116"/>
-      <c r="G120" s="117"/>
+      <c r="C120" s="117"/>
+      <c r="D120" s="117"/>
+      <c r="E120" s="117"/>
+      <c r="F120" s="117"/>
+      <c r="G120" s="118"/>
     </row>
     <row r="121" spans="1:7" ht="12.75" customHeight="1">
       <c r="A121" s="28"/>
-      <c r="B121" s="113" t="s">
+      <c r="B121" s="116" t="s">
         <v>484</v>
       </c>
-      <c r="C121" s="116"/>
-      <c r="D121" s="116"/>
-      <c r="E121" s="116"/>
-      <c r="F121" s="116"/>
-      <c r="G121" s="117"/>
+      <c r="C121" s="117"/>
+      <c r="D121" s="117"/>
+      <c r="E121" s="117"/>
+      <c r="F121" s="117"/>
+      <c r="G121" s="118"/>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="28"/>
@@ -5657,14 +5693,14 @@
       <c r="A136" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B136" s="113" t="s">
+      <c r="B136" s="116" t="s">
         <v>380</v>
       </c>
-      <c r="C136" s="116"/>
-      <c r="D136" s="116"/>
-      <c r="E136" s="116"/>
-      <c r="F136" s="116"/>
-      <c r="G136" s="117"/>
+      <c r="C136" s="117"/>
+      <c r="D136" s="117"/>
+      <c r="E136" s="117"/>
+      <c r="F136" s="117"/>
+      <c r="G136" s="118"/>
     </row>
     <row r="137" spans="1:7">
       <c r="A137" s="28"/>
@@ -5747,14 +5783,14 @@
       <c r="A142" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B142" s="113" t="s">
+      <c r="B142" s="116" t="s">
         <v>386</v>
       </c>
-      <c r="C142" s="116"/>
-      <c r="D142" s="116"/>
-      <c r="E142" s="116"/>
-      <c r="F142" s="116"/>
-      <c r="G142" s="117"/>
+      <c r="C142" s="117"/>
+      <c r="D142" s="117"/>
+      <c r="E142" s="117"/>
+      <c r="F142" s="117"/>
+      <c r="G142" s="118"/>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="28"/>
@@ -5828,14 +5864,14 @@
       <c r="A147" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B147" s="113" t="s">
+      <c r="B147" s="116" t="s">
         <v>389</v>
       </c>
-      <c r="C147" s="116"/>
-      <c r="D147" s="116"/>
-      <c r="E147" s="116"/>
-      <c r="F147" s="116"/>
-      <c r="G147" s="117"/>
+      <c r="C147" s="117"/>
+      <c r="D147" s="117"/>
+      <c r="E147" s="117"/>
+      <c r="F147" s="117"/>
+      <c r="G147" s="118"/>
     </row>
     <row r="148" spans="1:8" ht="13.5" customHeight="1">
       <c r="A148" s="28"/>
@@ -5909,14 +5945,14 @@
       <c r="A152" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B152" s="113" t="s">
+      <c r="B152" s="116" t="s">
         <v>389</v>
       </c>
-      <c r="C152" s="116"/>
-      <c r="D152" s="116"/>
-      <c r="E152" s="116"/>
-      <c r="F152" s="116"/>
-      <c r="G152" s="117"/>
+      <c r="C152" s="117"/>
+      <c r="D152" s="117"/>
+      <c r="E152" s="117"/>
+      <c r="F152" s="117"/>
+      <c r="G152" s="118"/>
     </row>
     <row r="153" spans="1:8" ht="13.5" customHeight="1">
       <c r="A153" s="28"/>
@@ -5928,7 +5964,7 @@
       <c r="G153" s="28"/>
     </row>
     <row r="154" spans="1:8">
-      <c r="A154" s="130" t="s">
+      <c r="A154" s="97" t="s">
         <v>560</v>
       </c>
       <c r="B154" s="49"/>
@@ -5978,7 +6014,7 @@
       <c r="F156" s="64" t="s">
         <v>566</v>
       </c>
-      <c r="G156" s="131" t="s">
+      <c r="G156" s="98" t="s">
         <v>567</v>
       </c>
     </row>
@@ -6013,29 +6049,29 @@
       <c r="G158" s="82"/>
     </row>
     <row r="159" spans="1:8">
-      <c r="A159" s="132" t="s">
+      <c r="A159" s="99" t="s">
         <v>315</v>
       </c>
-      <c r="B159" s="113" t="s">
+      <c r="B159" s="116" t="s">
         <v>572</v>
       </c>
-      <c r="C159" s="114"/>
-      <c r="D159" s="114"/>
-      <c r="E159" s="114"/>
-      <c r="F159" s="114"/>
-      <c r="G159" s="115"/>
+      <c r="C159" s="125"/>
+      <c r="D159" s="125"/>
+      <c r="E159" s="125"/>
+      <c r="F159" s="125"/>
+      <c r="G159" s="126"/>
       <c r="H159" s="93"/>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" s="28"/>
-      <c r="B160" s="113" t="s">
+      <c r="B160" s="116" t="s">
         <v>573</v>
       </c>
-      <c r="C160" s="114"/>
-      <c r="D160" s="114"/>
-      <c r="E160" s="114"/>
-      <c r="F160" s="114"/>
-      <c r="G160" s="115"/>
+      <c r="C160" s="125"/>
+      <c r="D160" s="125"/>
+      <c r="E160" s="125"/>
+      <c r="F160" s="125"/>
+      <c r="G160" s="126"/>
       <c r="H160" s="93"/>
     </row>
     <row r="161" spans="1:7">
@@ -6309,14 +6345,14 @@
       <c r="A175" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B175" s="124" t="s">
+      <c r="B175" s="119" t="s">
         <v>467</v>
       </c>
-      <c r="C175" s="125"/>
-      <c r="D175" s="125"/>
-      <c r="E175" s="125"/>
-      <c r="F175" s="125"/>
-      <c r="G175" s="126"/>
+      <c r="C175" s="120"/>
+      <c r="D175" s="120"/>
+      <c r="E175" s="120"/>
+      <c r="F175" s="120"/>
+      <c r="G175" s="121"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="30"/>
@@ -6511,14 +6547,14 @@
       <c r="A186" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B186" s="113" t="s">
+      <c r="B186" s="116" t="s">
         <v>455</v>
       </c>
-      <c r="C186" s="116"/>
-      <c r="D186" s="116"/>
-      <c r="E186" s="116"/>
-      <c r="F186" s="116"/>
-      <c r="G186" s="117"/>
+      <c r="C186" s="117"/>
+      <c r="D186" s="117"/>
+      <c r="E186" s="117"/>
+      <c r="F186" s="117"/>
+      <c r="G186" s="118"/>
     </row>
     <row r="187" spans="1:7" s="84" customFormat="1">
       <c r="A187" s="64"/>
@@ -6702,14 +6738,14 @@
       <c r="A197" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B197" s="124" t="s">
+      <c r="B197" s="119" t="s">
         <v>465</v>
       </c>
-      <c r="C197" s="125"/>
-      <c r="D197" s="125"/>
-      <c r="E197" s="125"/>
-      <c r="F197" s="125"/>
-      <c r="G197" s="126"/>
+      <c r="C197" s="120"/>
+      <c r="D197" s="120"/>
+      <c r="E197" s="120"/>
+      <c r="F197" s="120"/>
+      <c r="G197" s="121"/>
     </row>
     <row r="198" spans="1:7">
       <c r="A198" s="30"/>
@@ -6846,14 +6882,14 @@
       <c r="A205" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B205" s="124" t="s">
+      <c r="B205" s="119" t="s">
         <v>447</v>
       </c>
-      <c r="C205" s="125"/>
-      <c r="D205" s="125"/>
-      <c r="E205" s="125"/>
-      <c r="F205" s="125"/>
-      <c r="G205" s="126"/>
+      <c r="C205" s="120"/>
+      <c r="D205" s="120"/>
+      <c r="E205" s="120"/>
+      <c r="F205" s="120"/>
+      <c r="G205" s="121"/>
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="30"/>
@@ -6971,14 +7007,14 @@
       <c r="A212" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B212" s="113" t="s">
+      <c r="B212" s="116" t="s">
         <v>526</v>
       </c>
-      <c r="C212" s="116"/>
-      <c r="D212" s="116"/>
-      <c r="E212" s="116"/>
-      <c r="F212" s="116"/>
-      <c r="G212" s="117"/>
+      <c r="C212" s="117"/>
+      <c r="D212" s="117"/>
+      <c r="E212" s="117"/>
+      <c r="F212" s="117"/>
+      <c r="G212" s="118"/>
     </row>
     <row r="213" spans="1:7" ht="13.5" customHeight="1">
       <c r="A213" s="83"/>
@@ -7042,14 +7078,14 @@
       <c r="A217" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B217" s="124" t="s">
+      <c r="B217" s="119" t="s">
         <v>489</v>
       </c>
-      <c r="C217" s="125"/>
-      <c r="D217" s="125"/>
-      <c r="E217" s="125"/>
-      <c r="F217" s="125"/>
-      <c r="G217" s="126"/>
+      <c r="C217" s="120"/>
+      <c r="D217" s="120"/>
+      <c r="E217" s="120"/>
+      <c r="F217" s="120"/>
+      <c r="G217" s="121"/>
     </row>
     <row r="218" spans="1:7">
       <c r="A218" s="68"/>
@@ -7244,14 +7280,14 @@
       <c r="A228" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B228" s="113" t="s">
+      <c r="B228" s="116" t="s">
         <v>455</v>
       </c>
-      <c r="C228" s="116"/>
-      <c r="D228" s="116"/>
-      <c r="E228" s="116"/>
-      <c r="F228" s="116"/>
-      <c r="G228" s="117"/>
+      <c r="C228" s="117"/>
+      <c r="D228" s="117"/>
+      <c r="E228" s="117"/>
+      <c r="F228" s="117"/>
+      <c r="G228" s="118"/>
     </row>
     <row r="229" spans="1:7">
       <c r="A229" s="30"/>
@@ -7380,14 +7416,14 @@
       <c r="A236" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B236" s="113" t="s">
+      <c r="B236" s="116" t="s">
         <v>544</v>
       </c>
-      <c r="C236" s="116"/>
-      <c r="D236" s="116"/>
-      <c r="E236" s="116"/>
-      <c r="F236" s="116"/>
-      <c r="G236" s="117"/>
+      <c r="C236" s="117"/>
+      <c r="D236" s="117"/>
+      <c r="E236" s="117"/>
+      <c r="F236" s="117"/>
+      <c r="G236" s="118"/>
     </row>
     <row r="237" spans="1:7">
       <c r="A237" s="30"/>
@@ -7505,14 +7541,14 @@
       <c r="A243" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B243" s="113" t="s">
+      <c r="B243" s="116" t="s">
         <v>524</v>
       </c>
-      <c r="C243" s="116"/>
-      <c r="D243" s="116"/>
-      <c r="E243" s="116"/>
-      <c r="F243" s="116"/>
-      <c r="G243" s="117"/>
+      <c r="C243" s="117"/>
+      <c r="D243" s="117"/>
+      <c r="E243" s="117"/>
+      <c r="F243" s="117"/>
+      <c r="G243" s="118"/>
     </row>
     <row r="244" spans="1:8" ht="13.5" customHeight="1">
       <c r="A244" s="83"/>
@@ -7562,14 +7598,14 @@
       <c r="A247" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B247" s="113" t="s">
+      <c r="B247" s="116" t="s">
         <v>457</v>
       </c>
-      <c r="C247" s="116"/>
-      <c r="D247" s="116"/>
-      <c r="E247" s="116"/>
-      <c r="F247" s="116"/>
-      <c r="G247" s="117"/>
+      <c r="C247" s="117"/>
+      <c r="D247" s="117"/>
+      <c r="E247" s="117"/>
+      <c r="F247" s="117"/>
+      <c r="G247" s="118"/>
     </row>
     <row r="248" spans="1:8">
       <c r="A248" s="30"/>
@@ -7650,14 +7686,14 @@
       <c r="A253" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B253" s="113" t="s">
+      <c r="B253" s="116" t="s">
         <v>485</v>
       </c>
-      <c r="C253" s="116"/>
-      <c r="D253" s="116"/>
-      <c r="E253" s="116"/>
-      <c r="F253" s="116"/>
-      <c r="G253" s="117"/>
+      <c r="C253" s="117"/>
+      <c r="D253" s="117"/>
+      <c r="E253" s="117"/>
+      <c r="F253" s="117"/>
+      <c r="G253" s="118"/>
     </row>
     <row r="254" spans="1:8">
       <c r="A254" s="30"/>
@@ -7731,14 +7767,14 @@
       <c r="A258" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B258" s="113" t="s">
+      <c r="B258" s="116" t="s">
         <v>458</v>
       </c>
-      <c r="C258" s="116"/>
-      <c r="D258" s="116"/>
-      <c r="E258" s="116"/>
-      <c r="F258" s="116"/>
-      <c r="G258" s="117"/>
+      <c r="C258" s="117"/>
+      <c r="D258" s="117"/>
+      <c r="E258" s="117"/>
+      <c r="F258" s="117"/>
+      <c r="G258" s="118"/>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="30"/>
@@ -7814,26 +7850,36 @@
       <c r="A263" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="B263" s="113" t="s">
+      <c r="B263" s="116" t="s">
         <v>460</v>
       </c>
-      <c r="C263" s="116"/>
-      <c r="D263" s="116"/>
-      <c r="E263" s="116"/>
-      <c r="F263" s="116"/>
-      <c r="G263" s="117"/>
+      <c r="C263" s="117"/>
+      <c r="D263" s="117"/>
+      <c r="E263" s="117"/>
+      <c r="F263" s="117"/>
+      <c r="G263" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B247:G247"/>
-    <mergeCell ref="B253:G253"/>
-    <mergeCell ref="B258:G258"/>
-    <mergeCell ref="B263:G263"/>
-    <mergeCell ref="B197:G197"/>
-    <mergeCell ref="B205:G205"/>
-    <mergeCell ref="B243:G243"/>
-    <mergeCell ref="B212:G212"/>
-    <mergeCell ref="B236:G236"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B91:G91"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="B114:G114"/>
+    <mergeCell ref="B115:G115"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B152:G152"/>
+    <mergeCell ref="B121:G121"/>
+    <mergeCell ref="B136:G136"/>
+    <mergeCell ref="B142:G142"/>
+    <mergeCell ref="B147:G147"/>
+    <mergeCell ref="B159:G159"/>
+    <mergeCell ref="B160:G160"/>
     <mergeCell ref="B186:G186"/>
     <mergeCell ref="B228:G228"/>
     <mergeCell ref="B217:G217"/>
@@ -7850,25 +7896,15 @@
     <mergeCell ref="B72:G72"/>
     <mergeCell ref="B112:G112"/>
     <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B82:G82"/>
-    <mergeCell ref="B152:G152"/>
-    <mergeCell ref="B121:G121"/>
-    <mergeCell ref="B136:G136"/>
-    <mergeCell ref="B142:G142"/>
-    <mergeCell ref="B147:G147"/>
-    <mergeCell ref="B159:G159"/>
-    <mergeCell ref="B160:G160"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B91:G91"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="B114:G114"/>
-    <mergeCell ref="B115:G115"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B247:G247"/>
+    <mergeCell ref="B253:G253"/>
+    <mergeCell ref="B258:G258"/>
+    <mergeCell ref="B263:G263"/>
+    <mergeCell ref="B197:G197"/>
+    <mergeCell ref="B205:G205"/>
+    <mergeCell ref="B243:G243"/>
+    <mergeCell ref="B212:G212"/>
+    <mergeCell ref="B236:G236"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7879,10 +7915,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD89A094-B856-4791-AA7C-3560703CFD26}">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7891,192 +7927,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="133" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="134" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="134" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="134" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="134" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="134" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="134" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="134" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="134" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="134" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="134" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="134" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="134" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="134" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="134" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="134" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="134" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="134" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="134" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="134" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="134" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="134" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="134" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="134" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="134" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="134" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="134" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="134" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="30" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" s="134" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="30" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" s="134" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="30" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" s="134" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="30" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" s="134" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="30" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="134" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="30" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" s="134" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="30" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" s="134" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="30" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="134" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="30" t="s">
+    <row r="37" spans="1:1">
+      <c r="A37" s="134" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="30" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="135" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="30" t="s">
+    <row r="39" spans="1:1">
+      <c r="A39" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="30" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" s="2" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8477,24 +8523,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF3AC9B3629813499A0ACD8A875243EF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="922d0740f907dd86cb660748b16b5452">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2611df27-1940-46be-a00f-4132d3fec05a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbb66662760600521b39f06a97f3e4fa" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8683,10 +8711,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008A1C1A-9E5E-4F54-8085-06E04E5030EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBE8E031-5F32-4C4F-89D7-DA1D52DF419D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="2611df27-1940-46be-a00f-4132d3fec05a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8710,20 +8767,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBE8E031-5F32-4C4F-89D7-DA1D52DF419D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008A1C1A-9E5E-4F54-8085-06E04E5030EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="2611df27-1940-46be-a00f-4132d3fec05a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>